<commit_message>
WF Real. Past: CA,DR; Current: FE v004-v006
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Seguimiento Experimentos.xlsx
+++ b/src/workflow-colab/Seguimiento Experimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55855268-7CDB-493E-8EB9-33290FFD518F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C67808-770E-4EDB-8035-76DB77903E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{FE1D57DF-8E26-44DB-9048-BDF7AACEB845}"/>
+    <workbookView xWindow="38280" yWindow="3165" windowWidth="29040" windowHeight="15840" xr2:uid="{FE1D57DF-8E26-44DB-9048-BDF7AACEB845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Cota superior</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Semilla Canarios (L. 61)</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>FE.Corrido</t>
   </si>
 </sst>
 </file>
@@ -75,7 +81,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="000"/>
+    <numFmt numFmtId="165" formatCode="000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -119,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -208,6 +214,45 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -218,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,11 +288,18 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -564,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5618A040-37B5-4764-8ECE-E0692C50B903}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -580,7 +632,7 @@
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -602,8 +654,11 @@
       <c r="G1" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -626,8 +681,11 @@
         <f t="shared" ref="G2:G11" si="0">B2*2^C2</f>
         <v>320</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -650,8 +708,11 @@
         <f t="shared" si="0"/>
         <v>10240</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <f>A3+1</f>
         <v>3</v>
@@ -675,8 +736,9 @@
         <f t="shared" si="0"/>
         <v>10240</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <f t="shared" ref="A5:A11" si="1">A4+1</f>
         <v>4</v>
@@ -700,8 +762,9 @@
         <f t="shared" si="0"/>
         <v>10485760</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -725,8 +788,9 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -750,8 +814,9 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -775,8 +840,9 @@
         <f t="shared" si="0"/>
         <v>640</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -798,8 +864,9 @@
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -821,8 +888,9 @@
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -844,8 +912,9 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="16"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -856,7 +925,7 @@
         <v>108881</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
WF Real. arranca nuevamente. v006 a v010
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Seguimiento Experimentos.xlsx
+++ b/src/workflow-colab/Seguimiento Experimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C67808-770E-4EDB-8035-76DB77903E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D702743-044D-4375-A1EC-0CBF1C29F5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3165" windowWidth="29040" windowHeight="15840" xr2:uid="{FE1D57DF-8E26-44DB-9048-BDF7AACEB845}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{FE1D57DF-8E26-44DB-9048-BDF7AACEB845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Cota superior</t>
   </si>
@@ -619,7 +619,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +736,9 @@
         <f t="shared" si="0"/>
         <v>10240</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
@@ -788,7 +790,9 @@
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="12">

</xml_diff>

<commit_message>
primer zz: 202109 v006
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Seguimiento Experimentos.xlsx
+++ b/src/workflow-colab/Seguimiento Experimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F6628A-6697-4BBB-8E63-3263FE85362E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FC700-87B1-4438-9119-A3F68E40AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3165" windowWidth="29040" windowHeight="15840" xr2:uid="{FE1D57DF-8E26-44DB-9048-BDF7AACEB845}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>mtry</t>
   </si>
@@ -83,24 +83,6 @@
     <t>corriendo</t>
   </si>
   <si>
-    <t>631.start</t>
-  </si>
-  <si>
-    <t>631.finish</t>
-  </si>
-  <si>
-    <t>641.start</t>
-  </si>
-  <si>
-    <t>641.finish</t>
-  </si>
-  <si>
-    <t>631.T</t>
-  </si>
-  <si>
-    <t>641.T</t>
-  </si>
-  <si>
     <t>651.start</t>
   </si>
   <si>
@@ -108,16 +90,20 @@
   </si>
   <si>
     <t>651.T</t>
+  </si>
+  <si>
+    <t>imoggi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="000"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -278,23 +264,23 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,13 +288,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -320,13 +306,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -644,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5618A040-37B5-4764-8ECE-E0692C50B903}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -658,7 +644,7 @@
     <col min="7" max="7" width="4.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
@@ -684,43 +670,25 @@
         <v>13</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>12</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -740,15 +708,9 @@
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="18"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N2" s="18"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -776,15 +738,9 @@
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="18"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N3" s="18"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -812,15 +768,9 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="18"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N4" s="18"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <f>A4+1</f>
         <v>3</v>
@@ -849,15 +799,9 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="18"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <f t="shared" ref="A6:A12" si="0">A5+1</f>
         <v>4</v>
@@ -883,33 +827,21 @@
       <c r="H6" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19">
-        <f>IF(J6&lt;I6,TIME(24,0,0)+J6-I6,J6-I6)</f>
+      <c r="I6" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19">
+        <f>IF(L6&lt;K6,TIME(24,0,0)+L6-K6,L6-K6)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19">
-        <f>IF(N6&lt;M6,TIME(24,0,0)+N6-M6,N6-M6)</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19">
-        <f>IF(R6&lt;Q6,TIME(24,0,0)+R6-Q6,R6-Q6)</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="20"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N6" s="20"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -938,15 +870,9 @@
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="18"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -972,33 +898,23 @@
       <c r="H8" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19">
-        <f t="shared" ref="K8:K23" si="1">IF(J8&lt;I8,TIME(24,0,0)+J8-I8,J8-I8)</f>
+      <c r="I8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19">
+        <f t="shared" ref="M8:M23" si="1">IF(L8&lt;K8,TIME(24,0,0)+L8-K8,L8-K8)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19">
-        <f t="shared" ref="O8:O23" si="2">IF(N8&lt;M8,TIME(24,0,0)+N8-M8,N8-M8)</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19">
-        <f t="shared" ref="S8:S23" si="3">IF(R8&lt;Q8,TIME(24,0,0)+R8-Q8,R8-Q8)</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="20"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N8" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1024,33 +940,21 @@
       <c r="H9" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="23">
+      <c r="I9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="25">
         <f>TIME(13,52,0)</f>
         <v>0.57777777777777783</v>
       </c>
-      <c r="T9" s="20"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1076,33 +980,21 @@
       <c r="H10" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="23">
+      <c r="I10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="25">
         <f>TIME(7,15,0)</f>
         <v>0.30208333333333331</v>
       </c>
-      <c r="T10" s="20"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N10" s="20"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1128,35 +1020,23 @@
       <c r="H11" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19">
+      <c r="I11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="23">
+        <v>0.81041666666666667</v>
+      </c>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q11" s="24">
-        <v>0.81041666666666667</v>
-      </c>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19">
-        <f t="shared" si="3"/>
         <v>-0.81041666666666667</v>
       </c>
-      <c r="T11" s="20"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N11" s="20"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1182,35 +1062,23 @@
       <c r="H12" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21">
+      <c r="I12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q12" s="25">
-        <v>0.81111111111111101</v>
-      </c>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21">
-        <f t="shared" si="3"/>
         <v>-0.81111111111111101</v>
       </c>
-      <c r="T12" s="22"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N12" s="22"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>0</v>
       </c>
@@ -1230,15 +1098,9 @@
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="18"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>1</v>
       </c>
@@ -1266,15 +1128,9 @@
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="18"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N14" s="18"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>2</v>
       </c>
@@ -1302,15 +1158,9 @@
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="18"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <f>A15+1</f>
         <v>3</v>
@@ -1339,17 +1189,11 @@
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="18"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N16" s="18"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
-        <f t="shared" ref="A17:A23" si="4">A16+1</f>
+        <f t="shared" ref="A17:A23" si="2">A16+1</f>
         <v>4</v>
       </c>
       <c r="B17" s="7">
@@ -1371,29 +1215,17 @@
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
-      <c r="K17" s="19">
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19">
+      <c r="N17" s="20"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T17" s="20"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
-        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B18" s="11">
@@ -1420,17 +1252,11 @@
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="18"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="N18" s="18"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B19" s="7">
@@ -1454,41 +1280,31 @@
       <c r="H19" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19">
+      <c r="I19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L19" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19">
+      <c r="N19" s="20"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="20"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
-        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="B20" s="7">
         <v>202107</v>
       </c>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D20" s="9">
         <v>20</v>
       </c>
@@ -1501,38 +1317,34 @@
       <c r="G20" s="2">
         <v>20</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19">
+      <c r="H20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19">
+      <c r="N20" s="20"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="20"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="5">
-        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="B21" s="7">
         <v>202107</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D21" s="9">
         <v>30</v>
       </c>
@@ -1545,38 +1357,34 @@
       <c r="G21" s="2">
         <v>20</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19">
+      <c r="H21" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19">
+      <c r="N21" s="20"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T21" s="20"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="5">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="B22" s="7">
         <v>202107</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D22" s="9">
         <v>30</v>
       </c>
@@ -1589,38 +1397,34 @@
       <c r="G22" s="2">
         <v>20</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19">
+      <c r="H22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19">
+      <c r="N22" s="20"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T22" s="20"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="B23" s="8">
         <v>202107</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="D23" s="3">
         <v>50</v>
       </c>
@@ -1633,28 +1437,22 @@
       <c r="G23" s="4">
         <v>40</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21">
+      <c r="H23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="22"/>
+      <c r="N23" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>